<commit_message>
Added one more EDA test
</commit_message>
<xml_diff>
--- a/CH-095 Last Inventory.xlsx
+++ b/CH-095 Last Inventory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB8DF052-6CB3-4168-AE5A-DC14BCFAD338}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9DFAD45-1B2C-4452-AF9F-C27ED9B68B25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -110,7 +110,7 @@
     <t>https://www.linkedin.com/feed/update/urn:li:activity:7227780686835818497/</t>
   </si>
   <si>
-    <t>My work</t>
+    <t>Lookup alternative</t>
   </si>
 </sst>
 </file>
@@ -1219,7 +1219,7 @@
   <dimension ref="A1:T25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1541,9 +1541,14 @@
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11"/>
-      <c r="H11"/>
-      <c r="I11"/>
-      <c r="J11"/>
+      <c r="I11" s="1" t="str" cm="1">
+        <f t="array" ref="I11:I15">B3:B7</f>
+        <v>A</v>
+      </c>
+      <c r="J11" cm="1">
+        <f t="array" ref="J11">LOOKUP(2,1/(C3:G3&lt;&gt;""),C3:G3)</f>
+        <v>75</v>
+      </c>
       <c r="K11"/>
       <c r="L11" s="7"/>
       <c r="O11"/>
@@ -1560,9 +1565,13 @@
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12"/>
-      <c r="H12"/>
-      <c r="I12"/>
-      <c r="J12"/>
+      <c r="I12" t="str">
+        <v>B</v>
+      </c>
+      <c r="J12" cm="1">
+        <f t="array" ref="J12">LOOKUP(2,1/(C4:G4&lt;&gt;""),C4:G4)</f>
+        <v>80</v>
+      </c>
       <c r="K12"/>
       <c r="L12" s="8"/>
       <c r="O12"/>
@@ -1573,17 +1582,38 @@
       <c r="T12"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="I13" t="str">
+        <v>C</v>
+      </c>
+      <c r="J13" cm="1">
+        <f t="array" ref="J13">LOOKUP(2,1/(C5:G5&lt;&gt;""),C5:G5)</f>
+        <v>18</v>
+      </c>
       <c r="L13" s="8"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="I14" t="str">
+        <v>D</v>
+      </c>
+      <c r="J14" cm="1">
+        <f t="array" ref="J14">LOOKUP(2,1/(C6:G6&lt;&gt;""),C6:G6)</f>
+        <v>35</v>
+      </c>
       <c r="L14" s="8"/>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
+      <c r="I15" t="str">
+        <v>E</v>
+      </c>
+      <c r="J15" cm="1">
+        <f t="array" ref="J15">LOOKUP(2,1/(C7:G7&lt;&gt;""),C7:G7)</f>
+        <v>25</v>
+      </c>
       <c r="L15" s="8"/>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>

</xml_diff>

<commit_message>
My single function looks done
</commit_message>
<xml_diff>
--- a/CH-095 Last Inventory.xlsx
+++ b/CH-095 Last Inventory.xlsx
@@ -8,16 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9DFAD45-1B2C-4452-AF9F-C27ED9B68B25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63A8DA48-835B-4EB8-B082-C07B900CA365}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
     <sheet name="EDA" sheetId="2" r:id="rId2"/>
+    <sheet name="MySingleFunction" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">EDA!$B$3:$G$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">MySingleFunction!$B$3:$G$6</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$B$3:$G$6</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -63,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="17">
   <si>
     <t>Result</t>
   </si>
@@ -111,6 +113,9 @@
   </si>
   <si>
     <t>Lookup alternative</t>
+  </si>
+  <si>
+    <t>Index didn't work</t>
   </si>
 </sst>
 </file>
@@ -1218,8 +1223,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF40A59D-1856-4370-B4D6-8890433B0B63}">
   <dimension ref="A1:T25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1246,7 +1251,9 @@
       <c r="F1" s="17"/>
       <c r="G1" s="17"/>
       <c r="H1"/>
-      <c r="I1"/>
+      <c r="I1" t="s">
+        <v>16</v>
+      </c>
       <c r="J1"/>
       <c r="K1"/>
       <c r="M1" s="18" t="s">
@@ -1502,6 +1509,428 @@
       <c r="F9" s="3"/>
       <c r="G9"/>
       <c r="H9"/>
+      <c r="J9"/>
+      <c r="K9"/>
+      <c r="L9" s="7"/>
+      <c r="O9"/>
+      <c r="P9"/>
+      <c r="Q9"/>
+      <c r="R9"/>
+      <c r="S9"/>
+      <c r="T9"/>
+    </row>
+    <row r="10" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10"/>
+      <c r="H10"/>
+      <c r="I10" t="s">
+        <v>15</v>
+      </c>
+      <c r="J10"/>
+      <c r="K10"/>
+      <c r="L10" s="7"/>
+      <c r="O10"/>
+      <c r="P10"/>
+      <c r="Q10"/>
+      <c r="R10"/>
+      <c r="S10"/>
+      <c r="T10"/>
+    </row>
+    <row r="11" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11"/>
+      <c r="I11" s="1" t="str" cm="1">
+        <f t="array" ref="I11:I15">B3:B7</f>
+        <v>A</v>
+      </c>
+      <c r="J11" cm="1">
+        <f t="array" ref="J11">LOOKUP(2,1/(C3:G3&lt;&gt;""),C3:G3)</f>
+        <v>75</v>
+      </c>
+      <c r="K11"/>
+      <c r="L11" s="7"/>
+      <c r="O11"/>
+      <c r="P11"/>
+      <c r="Q11"/>
+      <c r="R11"/>
+      <c r="S11"/>
+      <c r="T11"/>
+    </row>
+    <row r="12" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12"/>
+      <c r="I12" t="str">
+        <v>B</v>
+      </c>
+      <c r="J12" cm="1">
+        <f t="array" ref="J12">LOOKUP(2,1/(C4:G4&lt;&gt;""),C4:G4)</f>
+        <v>80</v>
+      </c>
+      <c r="K12"/>
+      <c r="L12" s="8"/>
+      <c r="O12"/>
+      <c r="P12"/>
+      <c r="Q12"/>
+      <c r="R12"/>
+      <c r="S12"/>
+      <c r="T12"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="I13" t="str">
+        <v>C</v>
+      </c>
+      <c r="J13" cm="1">
+        <f t="array" ref="J13">LOOKUP(2,1/(C5:G5&lt;&gt;""),C5:G5)</f>
+        <v>18</v>
+      </c>
+      <c r="L13" s="8"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="I14" t="str">
+        <v>D</v>
+      </c>
+      <c r="J14" cm="1">
+        <f t="array" ref="J14">LOOKUP(2,1/(C6:G6&lt;&gt;""),C6:G6)</f>
+        <v>35</v>
+      </c>
+      <c r="L14" s="8"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="I15" t="str">
+        <v>E</v>
+      </c>
+      <c r="J15" cm="1">
+        <f t="array" ref="J15">LOOKUP(2,1/(C7:G7&lt;&gt;""),C7:G7)</f>
+        <v>25</v>
+      </c>
+      <c r="L15" s="8"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="L17" s="8"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="L18" s="8"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="L19" s="8"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="L20" s="1"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="L21" s="1"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="L22" s="1"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="L23" s="1"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L24" s="1"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L25" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="M1:N1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84949567-FC59-40DF-B79C-A7ED1EFC2DB6}">
+  <dimension ref="A1:T25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O16" sqref="O16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.09765625" customWidth="1"/>
+    <col min="2" max="2" width="10.59765625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="6.5" style="3" customWidth="1"/>
+    <col min="7" max="8" width="6.5" customWidth="1"/>
+    <col min="9" max="9" width="10.09765625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.5" customWidth="1"/>
+    <col min="12" max="12" width="4" customWidth="1"/>
+    <col min="13" max="13" width="9.59765625" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.19921875" style="4" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1"/>
+      <c r="I1"/>
+      <c r="J1"/>
+      <c r="K1"/>
+      <c r="M1" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="N1" s="18"/>
+      <c r="R1" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2"/>
+      <c r="I2"/>
+      <c r="J2"/>
+      <c r="K2"/>
+      <c r="M2" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="N2" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="13">
+        <v>89</v>
+      </c>
+      <c r="D3" s="13">
+        <v>83</v>
+      </c>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13">
+        <v>54</v>
+      </c>
+      <c r="G3" s="14">
+        <v>75</v>
+      </c>
+      <c r="H3" s="19"/>
+      <c r="I3"/>
+      <c r="J3"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="N3" s="13">
+        <v>75</v>
+      </c>
+      <c r="O3" s="9"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="9"/>
+      <c r="S3" s="9"/>
+      <c r="T3" s="7"/>
+    </row>
+    <row r="4" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="13">
+        <v>67</v>
+      </c>
+      <c r="D4" s="13">
+        <v>70</v>
+      </c>
+      <c r="E4" s="13">
+        <v>80</v>
+      </c>
+      <c r="F4" s="13"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="19"/>
+      <c r="I4"/>
+      <c r="J4"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="N4" s="13">
+        <v>80</v>
+      </c>
+      <c r="O4" s="9"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="9"/>
+      <c r="R4" s="9"/>
+      <c r="S4" s="9"/>
+      <c r="T4" s="7"/>
+    </row>
+    <row r="5" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="13">
+        <v>29</v>
+      </c>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13">
+        <v>67</v>
+      </c>
+      <c r="F5" s="13">
+        <v>18</v>
+      </c>
+      <c r="G5" s="14"/>
+      <c r="H5" s="19"/>
+      <c r="I5"/>
+      <c r="J5"/>
+      <c r="K5" s="19"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="N5" s="13">
+        <v>18</v>
+      </c>
+      <c r="O5" s="9"/>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="9"/>
+      <c r="R5" s="9"/>
+      <c r="S5" s="9"/>
+      <c r="T5" s="7"/>
+    </row>
+    <row r="6" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="13">
+        <v>18</v>
+      </c>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13">
+        <v>20</v>
+      </c>
+      <c r="F6" s="13"/>
+      <c r="G6" s="14">
+        <v>35</v>
+      </c>
+      <c r="H6" s="19"/>
+      <c r="I6"/>
+      <c r="J6"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="N6" s="13">
+        <v>35</v>
+      </c>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="9"/>
+      <c r="T6" s="7"/>
+    </row>
+    <row r="7" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="15">
+        <v>25</v>
+      </c>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="19"/>
+      <c r="I7"/>
+      <c r="J7"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="N7" s="15">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8"/>
+      <c r="H8"/>
+      <c r="I8"/>
+      <c r="J8"/>
+      <c r="K8"/>
+      <c r="L8" s="7"/>
+      <c r="O8"/>
+      <c r="P8"/>
+      <c r="Q8"/>
+      <c r="R8"/>
+      <c r="S8"/>
+      <c r="T8"/>
+    </row>
+    <row r="9" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9"/>
+      <c r="H9"/>
       <c r="I9" t="s">
         <v>15</v>
       </c>
@@ -1541,13 +1970,15 @@
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11"/>
-      <c r="I11" s="1" t="str" cm="1">
-        <f t="array" ref="I11:I15">B3:B7</f>
-        <v>A</v>
-      </c>
-      <c r="J11" cm="1">
-        <f t="array" ref="J11">LOOKUP(2,1/(C3:G3&lt;&gt;""),C3:G3)</f>
-        <v>75</v>
+      <c r="I11" s="12" t="str" cm="1">
+        <f t="array" ref="I11:J16">_xlfn.LET(
+_xlpm.z, _xlfn.BYROW(C3:G7,_xlfn.LAMBDA(_xlpm.r, LOOKUP(2,1/(_xlpm.r&lt;&gt;""),_xlpm.r))),
+_xlfn.VSTACK(M2:N2,_xlfn.HSTACK(B3:B7,_xlpm.z))
+)</f>
+        <v>Product</v>
+      </c>
+      <c r="J11" s="11" t="str">
+        <v>Last Inventory</v>
       </c>
       <c r="K11"/>
       <c r="L11" s="7"/>
@@ -1565,12 +1996,11 @@
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12"/>
-      <c r="I12" t="str">
-        <v>B</v>
-      </c>
-      <c r="J12" cm="1">
-        <f t="array" ref="J12">LOOKUP(2,1/(C4:G4&lt;&gt;""),C4:G4)</f>
-        <v>80</v>
+      <c r="I12" s="6" t="str">
+        <v>A</v>
+      </c>
+      <c r="J12" s="13">
+        <v>75</v>
       </c>
       <c r="K12"/>
       <c r="L12" s="8"/>
@@ -1582,24 +2012,22 @@
       <c r="T12"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="I13" t="str">
-        <v>C</v>
-      </c>
-      <c r="J13" cm="1">
-        <f t="array" ref="J13">LOOKUP(2,1/(C5:G5&lt;&gt;""),C5:G5)</f>
-        <v>18</v>
+      <c r="I13" s="6" t="str">
+        <v>B</v>
+      </c>
+      <c r="J13" s="13">
+        <v>80</v>
       </c>
       <c r="L13" s="8"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="I14" t="str">
-        <v>D</v>
-      </c>
-      <c r="J14" cm="1">
-        <f t="array" ref="J14">LOOKUP(2,1/(C6:G6&lt;&gt;""),C6:G6)</f>
-        <v>35</v>
+      <c r="I14" s="6" t="str">
+        <v>C</v>
+      </c>
+      <c r="J14" s="13">
+        <v>18</v>
       </c>
       <c r="L14" s="8"/>
       <c r="M14" s="2"/>
@@ -1607,12 +2035,11 @@
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
-      <c r="I15" t="str">
-        <v>E</v>
-      </c>
-      <c r="J15" cm="1">
-        <f t="array" ref="J15">LOOKUP(2,1/(C7:G7&lt;&gt;""),C7:G7)</f>
-        <v>25</v>
+      <c r="I15" s="6" t="str">
+        <v>D</v>
+      </c>
+      <c r="J15" s="13">
+        <v>35</v>
       </c>
       <c r="L15" s="8"/>
       <c r="M15" s="2"/>
@@ -1620,6 +2047,12 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
+      <c r="I16" s="10" t="str">
+        <v>E</v>
+      </c>
+      <c r="J16" s="15">
+        <v>25</v>
+      </c>
       <c r="L16" s="8"/>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>

</xml_diff>